<commit_message>
worked on the download sample functionality, also added a few fields to the forms
</commit_message>
<xml_diff>
--- a/frontend/pos/public/Sample.xlsx
+++ b/frontend/pos/public/Sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -38,6 +38,18 @@
   </si>
   <si>
     <t xml:space="preserve">Retail Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purchase Price </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min Retail Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max Retail Price </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min stock Qty</t>
   </si>
   <si>
     <t xml:space="preserve">Blue Pen</t>
@@ -162,13 +174,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -189,10 +201,22 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>100</v>
@@ -201,7 +225,7 @@
         <v>111121222</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>100</v>
@@ -209,25 +233,43 @@
       <c r="F2" s="2" t="n">
         <v>200</v>
       </c>
+      <c r="H2" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>1111144444</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <v>125</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>